<commit_message>
rebuild all derived docs
</commit_message>
<xml_diff>
--- a/docs/src/reference/data-dictionaries/Z_Dict.xlsx
+++ b/docs/src/reference/data-dictionaries/Z_Dict.xlsx
@@ -11298,7 +11298,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Spatial access to HCV Testing</t>
+          <t>Spatial access to Federally Qualified Health Centers (FQHCs)</t>
         </is>
       </c>
       <c r="C146" t="inlineStr"/>
@@ -11312,7 +11312,11 @@
       <c r="K146" t="inlineStr"/>
       <c r="L146" t="inlineStr"/>
       <c r="M146" t="inlineStr"/>
-      <c r="N146" t="inlineStr"/>
+      <c r="N146" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="O146" t="inlineStr"/>
       <c r="P146" t="inlineStr"/>
       <c r="Q146" t="inlineStr"/>
@@ -11326,28 +11330,28 @@
       <c r="U146" t="inlineStr"/>
       <c r="V146" t="inlineStr">
         <is>
-          <t>HcvCntDr</t>
+          <t>FqhcCntDr</t>
         </is>
       </c>
       <c r="W146" t="inlineStr">
         <is>
-          <t>Count of HCV Providers</t>
+          <t>Count of Federally Qualified Health Centers (FQHCs) within 30-min drive</t>
         </is>
       </c>
       <c r="X146" t="inlineStr"/>
       <c r="Y146" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_HCVTesting.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_FQHCs.md</t>
         </is>
       </c>
       <c r="Z146" t="inlineStr">
         <is>
-          <t>SAMHSA 2025</t>
+          <t>HRSA 2020 &amp; 2025; OSM 2019 &amp; 2025; Census TIGER 2018 &amp; 2020</t>
         </is>
       </c>
       <c r="AA146" t="inlineStr">
         <is>
-          <t>U.S. Substance Abuse and Mental Health Services Administration, Treatment Locator Tool, 2025</t>
+          <t>United States Covid Atlas via Health Resources and Services Adminsitration, 2020 &amp; 2025; Open Street Map 2019 &amp; 2025; Census Tiger/Line 2018 &amp; 2020 Shapefiles</t>
         </is>
       </c>
       <c r="AB146" t="inlineStr"/>
@@ -11362,7 +11366,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Spatial access to HCV Testing</t>
+          <t>Spatial access to Federally Qualified Health Centers (FQHCs)</t>
         </is>
       </c>
       <c r="C147" t="inlineStr"/>
@@ -11376,7 +11380,11 @@
       <c r="K147" t="inlineStr"/>
       <c r="L147" t="inlineStr"/>
       <c r="M147" t="inlineStr"/>
-      <c r="N147" t="inlineStr"/>
+      <c r="N147" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="O147" t="inlineStr"/>
       <c r="P147" t="inlineStr"/>
       <c r="Q147" t="inlineStr"/>
@@ -11390,28 +11398,28 @@
       <c r="U147" t="inlineStr"/>
       <c r="V147" t="inlineStr">
         <is>
-          <t>HcvMinDis</t>
+          <t>FqhcMinDis</t>
         </is>
       </c>
       <c r="W147" t="inlineStr">
         <is>
-          <t>Distance to nearest HCV Provider</t>
+          <t>Distance (mi) to nearest Federally Qualified Health Centers (FQHC)</t>
         </is>
       </c>
       <c r="X147" t="inlineStr"/>
       <c r="Y147" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_HCVTesting.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_FQHCs.md</t>
         </is>
       </c>
       <c r="Z147" t="inlineStr">
         <is>
-          <t>SAMHSA 2025</t>
+          <t>HRSA 2020 &amp; 2025; OSM 2019 &amp; 2025; Census TIGER 2018 &amp; 2020</t>
         </is>
       </c>
       <c r="AA147" t="inlineStr">
         <is>
-          <t>U.S. Substance Abuse and Mental Health Services Administration, Treatment Locator Tool, 2025</t>
+          <t>United States Covid Atlas via Health Resources and Services Adminsitration, 2020 &amp; 2025; Open Street Map 2019 &amp; 2025; Census Tiger/Line 2018 &amp; 2020 Shapefiles</t>
         </is>
       </c>
       <c r="AB147" t="inlineStr"/>
@@ -11426,7 +11434,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Spatial access to HCV Testing</t>
+          <t>Spatial access to Federally Qualified Health Centers (FQHCs)</t>
         </is>
       </c>
       <c r="C148" t="inlineStr"/>
@@ -11440,7 +11448,11 @@
       <c r="K148" t="inlineStr"/>
       <c r="L148" t="inlineStr"/>
       <c r="M148" t="inlineStr"/>
-      <c r="N148" t="inlineStr"/>
+      <c r="N148" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="O148" t="inlineStr"/>
       <c r="P148" t="inlineStr"/>
       <c r="Q148" t="inlineStr"/>
@@ -11450,32 +11462,36 @@
           <t>x</t>
         </is>
       </c>
-      <c r="T148" t="inlineStr"/>
+      <c r="T148" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="U148" t="inlineStr"/>
       <c r="V148" t="inlineStr">
         <is>
-          <t>HcvTmDr</t>
+          <t>FqhcTmDr</t>
         </is>
       </c>
       <c r="W148" t="inlineStr">
         <is>
-          <t>Driving time to nearest HCV Provider</t>
+          <t>Driving time (min) to nearest Federally Qualified Health Centers (FQHC)</t>
         </is>
       </c>
       <c r="X148" t="inlineStr"/>
       <c r="Y148" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_HCVTesting.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_FQHCs.md</t>
         </is>
       </c>
       <c r="Z148" t="inlineStr">
         <is>
-          <t>SAMHSA 2025</t>
+          <t>HRSA 2020 &amp; 2025; OSM 2019 &amp; 2025; Census TIGER 2018 &amp; 2020</t>
         </is>
       </c>
       <c r="AA148" t="inlineStr">
         <is>
-          <t>U.S. Substance Abuse and Mental Health Services Administration, Treatment Locator Tool, 2025</t>
+          <t>United States Covid Atlas via Health Resources and Services Adminsitration, 2020 &amp; 2025; Open Street Map 2019 &amp; 2025; Census Tiger/Line 2018 &amp; 2020 Shapefiles</t>
         </is>
       </c>
       <c r="AB148" t="inlineStr"/>
@@ -11518,12 +11534,12 @@
       <c r="U149" t="inlineStr"/>
       <c r="V149" t="inlineStr">
         <is>
-          <t>HivCntDr</t>
+          <t>HcvCntDr</t>
         </is>
       </c>
       <c r="W149" t="inlineStr">
         <is>
-          <t>Count of HIV Providers</t>
+          <t>Count of HCV Providers</t>
         </is>
       </c>
       <c r="X149" t="inlineStr"/>
@@ -11582,12 +11598,12 @@
       <c r="U150" t="inlineStr"/>
       <c r="V150" t="inlineStr">
         <is>
-          <t>HivMinDis</t>
+          <t>HcvMinDis</t>
         </is>
       </c>
       <c r="W150" t="inlineStr">
         <is>
-          <t>Distance to nearest HIV Provider</t>
+          <t>Distance to nearest HCV Provider</t>
         </is>
       </c>
       <c r="X150" t="inlineStr"/>
@@ -11646,12 +11662,12 @@
       <c r="U151" t="inlineStr"/>
       <c r="V151" t="inlineStr">
         <is>
-          <t>HivTmDr</t>
+          <t>HcvTmDr</t>
         </is>
       </c>
       <c r="W151" t="inlineStr">
         <is>
-          <t>Driving time to nearest HIV Provider</t>
+          <t>Driving time to nearest HCV Provider</t>
         </is>
       </c>
       <c r="X151" t="inlineStr"/>
@@ -11682,7 +11698,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Spatial access to Health Centers</t>
+          <t>Spatial access to HCV Testing</t>
         </is>
       </c>
       <c r="C152" t="inlineStr"/>
@@ -11696,11 +11712,7 @@
       <c r="K152" t="inlineStr"/>
       <c r="L152" t="inlineStr"/>
       <c r="M152" t="inlineStr"/>
-      <c r="N152" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="N152" t="inlineStr"/>
       <c r="O152" t="inlineStr"/>
       <c r="P152" t="inlineStr"/>
       <c r="Q152" t="inlineStr"/>
@@ -11714,28 +11726,28 @@
       <c r="U152" t="inlineStr"/>
       <c r="V152" t="inlineStr">
         <is>
-          <t>FqhcCntDr</t>
+          <t>HivCntDr</t>
         </is>
       </c>
       <c r="W152" t="inlineStr">
         <is>
-          <t>Count of FQHCs (30-min drive)</t>
+          <t>Count of HIV Providers</t>
         </is>
       </c>
       <c r="X152" t="inlineStr"/>
       <c r="Y152" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_FQHCs.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_HCVTesting.md</t>
         </is>
       </c>
       <c r="Z152" t="inlineStr">
         <is>
-          <t>US Covid Atlas via HRSA 2020; Tiger/Line 2018</t>
+          <t>SAMHSA 2025</t>
         </is>
       </c>
       <c r="AA152" t="inlineStr">
         <is>
-          <t>United States Covid Atlas via Health Resources and Services Adminsitration, 2020; Tiger/Line 2018 Shapefiles</t>
+          <t>U.S. Substance Abuse and Mental Health Services Administration, Treatment Locator Tool, 2025</t>
         </is>
       </c>
       <c r="AB152" t="inlineStr"/>
@@ -11750,7 +11762,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Spatial access to Health Centers</t>
+          <t>Spatial access to HCV Testing</t>
         </is>
       </c>
       <c r="C153" t="inlineStr"/>
@@ -11764,11 +11776,7 @@
       <c r="K153" t="inlineStr"/>
       <c r="L153" t="inlineStr"/>
       <c r="M153" t="inlineStr"/>
-      <c r="N153" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="N153" t="inlineStr"/>
       <c r="O153" t="inlineStr"/>
       <c r="P153" t="inlineStr"/>
       <c r="Q153" t="inlineStr"/>
@@ -11782,28 +11790,28 @@
       <c r="U153" t="inlineStr"/>
       <c r="V153" t="inlineStr">
         <is>
-          <t>FqhcMinDis</t>
+          <t>HivMinDis</t>
         </is>
       </c>
       <c r="W153" t="inlineStr">
         <is>
-          <t>Distance (mi) to nearest FQHC</t>
+          <t>Distance to nearest HIV Provider</t>
         </is>
       </c>
       <c r="X153" t="inlineStr"/>
       <c r="Y153" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_FQHCs.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_HCVTesting.md</t>
         </is>
       </c>
       <c r="Z153" t="inlineStr">
         <is>
-          <t>US Covid Atlas via HRSA 2020; Tiger/Line 2018</t>
+          <t>SAMHSA 2025</t>
         </is>
       </c>
       <c r="AA153" t="inlineStr">
         <is>
-          <t>United States Covid Atlas via Health Resources and Services Adminsitration, 2020; Tiger/Line 2018 Shapefiles</t>
+          <t>U.S. Substance Abuse and Mental Health Services Administration, Treatment Locator Tool, 2025</t>
         </is>
       </c>
       <c r="AB153" t="inlineStr"/>
@@ -11818,7 +11826,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Spatial access to Health Centers</t>
+          <t>Spatial access to HCV Testing</t>
         </is>
       </c>
       <c r="C154" t="inlineStr"/>
@@ -11832,11 +11840,7 @@
       <c r="K154" t="inlineStr"/>
       <c r="L154" t="inlineStr"/>
       <c r="M154" t="inlineStr"/>
-      <c r="N154" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="N154" t="inlineStr"/>
       <c r="O154" t="inlineStr"/>
       <c r="P154" t="inlineStr"/>
       <c r="Q154" t="inlineStr"/>
@@ -11846,36 +11850,32 @@
           <t>x</t>
         </is>
       </c>
-      <c r="T154" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="T154" t="inlineStr"/>
       <c r="U154" t="inlineStr"/>
       <c r="V154" t="inlineStr">
         <is>
-          <t>FqhcTmDr</t>
+          <t>HivTmDr</t>
         </is>
       </c>
       <c r="W154" t="inlineStr">
         <is>
-          <t>Driving time (min) to nearest FQHC</t>
+          <t>Driving time to nearest HIV Provider</t>
         </is>
       </c>
       <c r="X154" t="inlineStr"/>
       <c r="Y154" t="inlineStr">
         <is>
-          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_FQHCs.md</t>
+          <t>https://github.com/healthyregions/oeps/blob/main/metadata/Access_HCVTesting.md</t>
         </is>
       </c>
       <c r="Z154" t="inlineStr">
         <is>
-          <t>US Covid Atlas via HRSA 2020; Tiger/Line 2018</t>
+          <t>SAMHSA 2025</t>
         </is>
       </c>
       <c r="AA154" t="inlineStr">
         <is>
-          <t>United States Covid Atlas via Health Resources and Services Adminsitration, 2020; Tiger/Line 2018 Shapefiles</t>
+          <t>U.S. Substance Abuse and Mental Health Services Administration, Treatment Locator Tool, 2025</t>
         </is>
       </c>
       <c r="AB154" t="inlineStr"/>

</xml_diff>